<commit_message>
need to edit selectors
</commit_message>
<xml_diff>
--- a/Data/Repo.xlsx
+++ b/Data/Repo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ckat\Documents\UiPath\uipath-automation-5\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\revature-workspace\uipath-automation-5\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA1164D-5E2C-4ECF-9F53-2298812819D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259FD6BA-1D45-48A2-B3B6-EB3B2B4860B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7215" yWindow="2865" windowWidth="14550" windowHeight="10740" xr2:uid="{7018022E-AB31-4D1E-9D9C-0A4F52EE9788}"/>
+    <workbookView xWindow="7080" yWindow="3735" windowWidth="21600" windowHeight="11385" xr2:uid="{7018022E-AB31-4D1E-9D9C-0A4F52EE9788}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,21 +34,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Repository</t>
+    <t>https://github.com/antonyt96/TestRepo1</t>
   </si>
   <si>
-    <t>https://github.com/schigit/anotherrepo</t>
+    <t>https://github.com/antonyt96/TestRepo3</t>
   </si>
   <si>
-    <t>https://github.com/schigit/yetanothertestrepo</t>
+    <t>https://github.com/antonyt96/TestRepo2</t>
   </si>
   <si>
-    <t>https://github.com/schigit/testrepo</t>
-  </si>
-  <si>
-    <t>https://github.com/schigit/anothertestrepo</t>
+    <t>Repository URL</t>
   </si>
 </sst>
 </file>
@@ -413,9 +410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1863D87B-84CD-406A-A214-69FC679D6108}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -424,12 +419,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -439,20 +434,17 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{55A4B271-89D7-4FFF-89DA-FC4457232CA5}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{1412876E-0FC9-4E63-A796-66ED37EAD072}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{85B6C538-5531-4F06-89E8-FCCFEC683B90}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{BAE1F388-9FF8-48E5-BF24-CFBA2760C715}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>